<commit_message>
added - velocity/acceleration/jerk on the y axis
</commit_message>
<xml_diff>
--- a/analyses/data/pilotData_101_kin.xlsx
+++ b/analyses/data/pilotData_101_kin.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55968" uniqueCount="13992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97944" uniqueCount="13992">
   <si>
     <t>StimDuration</t>
   </si>
@@ -42009,7 +42009,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="956">
+  <borders count="1910">
     <border>
       <left/>
       <right/>
@@ -42972,11 +42972,965 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="956">
+  <cellXfs count="1910">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -43933,6 +44887,960 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="953" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="954" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="955" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="956" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="957" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="958" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="959" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="960" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="961" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="962" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="963" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="964" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="965" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="966" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="967" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="968" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="969" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="970" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="971" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="972" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="973" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="974" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="975" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="976" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="977" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="978" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="979" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="980" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="981" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="982" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="983" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="984" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="985" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="986" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="987" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="988" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="989" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="990" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="991" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="992" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="993" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="994" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="995" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="996" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="997" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="998" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="999" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1000" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1001" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1002" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1003" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1004" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1005" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1006" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1007" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1008" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1009" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1010" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1011" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1012" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1013" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1014" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1015" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1016" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1017" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1018" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1019" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1020" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1021" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1022" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1023" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1024" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1025" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1026" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1027" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1028" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1029" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1030" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1031" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1032" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1033" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1034" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1035" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1036" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1037" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1038" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1039" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1040" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1041" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1042" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1043" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1044" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1045" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1046" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1047" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1048" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1049" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1050" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1051" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1052" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1053" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1054" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1055" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1056" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1057" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1058" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1059" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1060" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1061" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1062" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1063" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1064" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1065" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1066" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1067" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1068" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1069" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1070" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1071" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1072" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1073" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1074" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1075" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1076" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1077" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1078" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1079" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1080" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1081" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1082" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1083" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1084" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1085" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1086" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1087" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1088" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1089" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1090" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1091" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1092" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1093" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1094" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1095" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1096" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1097" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1098" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1099" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1100" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1101" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1102" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1103" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1104" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1105" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1106" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1107" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1108" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1109" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1110" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1111" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1112" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1113" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1114" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1115" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1116" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1117" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1118" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1119" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1120" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1121" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1122" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1123" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1124" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1125" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1126" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1127" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1128" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1129" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1130" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1131" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1132" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1133" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1134" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1135" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1136" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1137" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1138" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1139" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1140" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1141" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1142" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1143" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1144" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1145" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1146" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1147" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1148" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1149" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1150" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1151" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1152" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1153" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1154" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1155" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1156" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1157" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1158" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1159" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1160" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1161" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1162" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1163" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1164" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1165" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1166" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1167" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1168" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1169" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1170" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1171" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1172" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1173" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1174" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1175" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1176" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1177" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1178" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1179" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1180" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1181" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1182" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1183" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1184" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1185" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1186" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1187" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1188" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1189" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1190" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1191" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1192" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1193" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1194" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1195" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1196" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1197" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1198" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1199" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1200" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1201" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1202" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1203" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1204" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1205" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1206" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1207" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1208" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1209" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1210" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1211" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1212" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1213" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1214" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1215" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1216" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1217" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1218" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1219" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1220" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1221" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1222" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1223" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1224" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1225" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1226" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1227" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1228" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1229" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1230" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1231" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1232" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1233" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1234" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1235" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1236" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1237" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1238" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1239" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1240" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1241" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1242" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1243" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1244" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1245" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1246" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1247" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1248" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1249" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1250" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1251" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1252" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1253" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1254" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1255" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1256" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1257" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1258" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1259" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1260" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1261" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1262" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1263" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1264" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1265" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1266" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1267" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1268" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1269" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1270" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1271" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1272" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1273" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1274" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1275" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1276" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1277" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1278" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1279" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1280" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1281" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1282" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1283" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1284" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1285" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1286" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1287" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1288" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1289" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1290" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1291" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1292" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1293" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1294" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1295" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1296" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1297" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1298" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1299" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1300" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1301" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1302" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1303" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1304" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1305" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1306" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1307" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1308" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1309" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1310" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1311" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1312" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1313" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1314" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1315" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1316" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1317" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1318" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1319" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1320" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1321" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1322" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1323" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1324" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1325" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1326" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1327" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1328" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1329" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1330" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1331" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1332" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1333" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1334" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1335" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1336" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1337" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1338" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1339" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1340" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1341" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1342" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1343" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1344" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1345" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1346" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1347" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1348" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1349" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1350" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1351" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1352" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1353" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1354" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1355" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1356" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1357" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1358" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1359" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1360" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1361" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1362" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1363" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1364" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1365" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1366" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1367" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1368" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1369" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1370" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1371" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1372" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1373" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1374" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1375" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1376" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1377" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1378" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1379" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1380" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1381" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1382" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1383" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1384" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1385" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1386" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1387" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1388" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1389" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1390" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1391" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1392" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1393" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1394" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1395" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1396" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1397" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1398" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1399" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1400" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1401" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1402" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1403" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1404" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1405" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1406" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1407" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1408" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1409" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1410" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1411" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1412" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1413" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1414" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1415" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1416" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1417" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1418" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1419" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1420" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1421" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1422" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1423" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1424" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1425" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1426" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1427" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1428" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1429" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1430" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1431" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1432" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1433" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1434" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1435" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1436" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1437" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1438" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1439" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1440" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1441" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1442" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1443" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1444" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1445" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1446" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1447" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1448" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1449" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1450" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1451" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1452" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1453" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1454" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1455" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1456" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1457" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1458" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1459" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1460" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1461" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1462" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1463" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1464" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1465" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1466" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1467" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1468" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1469" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1470" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1471" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1472" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1473" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1474" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1475" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1476" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1477" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1478" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1479" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1480" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1481" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1482" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1483" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1484" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1485" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1486" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1487" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1488" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1489" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1490" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1491" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1492" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1493" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1494" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1495" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1496" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1497" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1498" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1499" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1500" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1501" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1502" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1503" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1504" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1505" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1506" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1507" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1508" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1509" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1510" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1511" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1512" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1513" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1514" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1515" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1516" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1517" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1518" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1519" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1520" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1521" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1522" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1523" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1524" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1525" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1526" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1527" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1528" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1529" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1530" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1531" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1532" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1533" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1534" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1535" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1536" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1537" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1538" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1539" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1540" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1541" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1542" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1543" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1544" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1545" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1546" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1547" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1548" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1549" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1550" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1551" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1552" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1553" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1554" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1555" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1556" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1557" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1558" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1559" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1560" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1561" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1562" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1563" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1564" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1565" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1566" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1567" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1568" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1569" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1570" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1571" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1572" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1573" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1574" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1575" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1576" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1577" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1578" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1579" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1580" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1581" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1582" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1583" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1584" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1585" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1586" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1587" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1588" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1589" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1590" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1591" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1592" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1593" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1594" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1595" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1596" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1597" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1598" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1599" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1600" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1601" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1602" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1603" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1604" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1605" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1606" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1607" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1608" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1609" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1610" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1611" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1612" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1613" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1614" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1615" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1616" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1617" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1618" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1619" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1620" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1621" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1622" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1623" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1624" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1625" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1626" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1627" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1628" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1629" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1630" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1631" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1632" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1633" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1634" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1635" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1636" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1637" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1638" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1639" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1640" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1641" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1642" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1643" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1644" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1645" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1646" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1647" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1648" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1649" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1650" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1651" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1652" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1653" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1654" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1655" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1656" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1657" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1658" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1659" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1660" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1661" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1662" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1663" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1664" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1665" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1666" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1667" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1668" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1669" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1670" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1671" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1672" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1673" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1674" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1675" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1676" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1677" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1678" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1679" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1680" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1681" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1682" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1683" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1684" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1685" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1686" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1687" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1688" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1689" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1690" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1691" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1692" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1693" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1694" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1695" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1696" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1697" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1698" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1699" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1700" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1701" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1702" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1703" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1704" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1705" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1706" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1707" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1708" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1709" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1710" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1711" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1712" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1713" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1714" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1715" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1716" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1717" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1718" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1719" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1720" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1721" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1722" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1723" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1724" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1725" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1726" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1727" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1728" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1729" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1730" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1731" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1732" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1733" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1734" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1735" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1736" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1737" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1738" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1739" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1740" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1741" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1742" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1743" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1744" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1745" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1746" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1747" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1748" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1749" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1750" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1751" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1752" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1753" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1754" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1755" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1756" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1757" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1758" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1759" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1760" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1761" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1762" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1763" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1764" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1765" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1766" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1767" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1768" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1769" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1770" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1771" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1772" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1773" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1774" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1775" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1776" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1777" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1778" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1779" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1780" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1781" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1782" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1783" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1784" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1785" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1786" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1787" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1788" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1789" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1790" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1791" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1792" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1793" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1794" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1795" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1796" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1797" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1798" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1799" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1800" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1801" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1802" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1803" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1804" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1805" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1806" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1807" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1808" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1809" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1810" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1811" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1812" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1813" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1814" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1815" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1816" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1817" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1818" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1819" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1820" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1821" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1822" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1823" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1824" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1825" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1826" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1827" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1828" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1829" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1830" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1831" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1832" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1833" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1834" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1835" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1836" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1837" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1838" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1839" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1840" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1841" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1842" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1843" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1844" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1845" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1846" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1847" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1848" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1849" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1850" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1851" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1852" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1853" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1854" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1855" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1856" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1857" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1858" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1859" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1860" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1861" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1862" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1863" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1864" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1865" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1866" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1867" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1868" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1869" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1870" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1871" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1872" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1873" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1874" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1875" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1876" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1877" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1878" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1879" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1880" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1881" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1882" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1883" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1884" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1885" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1886" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1887" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1888" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1889" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1890" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1891" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1892" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1893" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1894" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1895" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1896" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1897" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1898" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1899" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1900" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1901" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1902" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1903" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1904" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1905" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1906" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1907" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1908" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1909" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -44036,268 +45944,268 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="954" t="s">
+      <c r="A1" s="1908" t="s">
         <v>13904</v>
       </c>
-      <c r="B1" s="954" t="s">
+      <c r="B1" s="1908" t="s">
         <v>13905</v>
       </c>
-      <c r="C1" s="954" t="s">
+      <c r="C1" s="1908" t="s">
         <v>13906</v>
       </c>
-      <c r="D1" s="954" t="s">
+      <c r="D1" s="1908" t="s">
         <v>13907</v>
       </c>
-      <c r="E1" s="954" t="s">
+      <c r="E1" s="1908" t="s">
         <v>13908</v>
       </c>
-      <c r="F1" s="954" t="s">
+      <c r="F1" s="1908" t="s">
         <v>13909</v>
       </c>
-      <c r="G1" s="954" t="s">
+      <c r="G1" s="1908" t="s">
         <v>13910</v>
       </c>
-      <c r="H1" s="954" t="s">
+      <c r="H1" s="1908" t="s">
         <v>13911</v>
       </c>
-      <c r="I1" s="954" t="s">
+      <c r="I1" s="1908" t="s">
         <v>13912</v>
       </c>
-      <c r="J1" s="954" t="s">
+      <c r="J1" s="1908" t="s">
         <v>13913</v>
       </c>
-      <c r="K1" s="954" t="s">
+      <c r="K1" s="1908" t="s">
         <v>13914</v>
       </c>
-      <c r="L1" s="954" t="s">
+      <c r="L1" s="1908" t="s">
         <v>13915</v>
       </c>
-      <c r="M1" s="954" t="s">
+      <c r="M1" s="1908" t="s">
         <v>13916</v>
       </c>
-      <c r="N1" s="954" t="s">
+      <c r="N1" s="1908" t="s">
         <v>13917</v>
       </c>
-      <c r="O1" s="954" t="s">
+      <c r="O1" s="1908" t="s">
         <v>13918</v>
       </c>
-      <c r="P1" s="954" t="s">
+      <c r="P1" s="1908" t="s">
         <v>13919</v>
       </c>
-      <c r="Q1" s="954" t="s">
+      <c r="Q1" s="1908" t="s">
         <v>13920</v>
       </c>
-      <c r="R1" s="954" t="s">
+      <c r="R1" s="1908" t="s">
         <v>13921</v>
       </c>
-      <c r="S1" s="954" t="s">
+      <c r="S1" s="1908" t="s">
         <v>13922</v>
       </c>
-      <c r="T1" s="954" t="s">
+      <c r="T1" s="1908" t="s">
         <v>13923</v>
       </c>
-      <c r="U1" s="954" t="s">
+      <c r="U1" s="1908" t="s">
         <v>13924</v>
       </c>
-      <c r="V1" s="954" t="s">
+      <c r="V1" s="1908" t="s">
         <v>13925</v>
       </c>
-      <c r="W1" s="954" t="s">
+      <c r="W1" s="1908" t="s">
         <v>13926</v>
       </c>
-      <c r="X1" s="954" t="s">
+      <c r="X1" s="1908" t="s">
         <v>13927</v>
       </c>
-      <c r="Y1" s="954" t="s">
+      <c r="Y1" s="1908" t="s">
         <v>13928</v>
       </c>
-      <c r="Z1" s="954" t="s">
+      <c r="Z1" s="1908" t="s">
         <v>13929</v>
       </c>
-      <c r="AA1" s="954" t="s">
+      <c r="AA1" s="1908" t="s">
         <v>13930</v>
       </c>
-      <c r="AB1" s="954" t="s">
+      <c r="AB1" s="1908" t="s">
         <v>13931</v>
       </c>
-      <c r="AC1" s="954" t="s">
+      <c r="AC1" s="1908" t="s">
         <v>13932</v>
       </c>
-      <c r="AD1" s="954" t="s">
+      <c r="AD1" s="1908" t="s">
         <v>13933</v>
       </c>
-      <c r="AE1" s="954" t="s">
+      <c r="AE1" s="1908" t="s">
         <v>13934</v>
       </c>
-      <c r="AF1" s="954" t="s">
+      <c r="AF1" s="1908" t="s">
         <v>13935</v>
       </c>
-      <c r="AG1" s="954" t="s">
+      <c r="AG1" s="1908" t="s">
         <v>13936</v>
       </c>
-      <c r="AH1" s="954" t="s">
+      <c r="AH1" s="1908" t="s">
         <v>13937</v>
       </c>
-      <c r="AI1" s="954" t="s">
+      <c r="AI1" s="1908" t="s">
         <v>13938</v>
       </c>
-      <c r="AJ1" s="954" t="s">
+      <c r="AJ1" s="1908" t="s">
         <v>13939</v>
       </c>
-      <c r="AK1" s="954" t="s">
+      <c r="AK1" s="1908" t="s">
         <v>13940</v>
       </c>
-      <c r="AL1" s="954" t="s">
+      <c r="AL1" s="1908" t="s">
         <v>13941</v>
       </c>
-      <c r="AM1" s="954" t="s">
+      <c r="AM1" s="1908" t="s">
         <v>13942</v>
       </c>
-      <c r="AN1" s="954" t="s">
+      <c r="AN1" s="1908" t="s">
         <v>13943</v>
       </c>
-      <c r="AO1" s="954" t="s">
+      <c r="AO1" s="1908" t="s">
         <v>13944</v>
       </c>
-      <c r="AP1" s="954" t="s">
+      <c r="AP1" s="1908" t="s">
         <v>13945</v>
       </c>
-      <c r="AQ1" s="954" t="s">
+      <c r="AQ1" s="1908" t="s">
         <v>13946</v>
       </c>
-      <c r="AR1" s="954" t="s">
+      <c r="AR1" s="1908" t="s">
         <v>13947</v>
       </c>
-      <c r="AS1" s="954" t="s">
+      <c r="AS1" s="1908" t="s">
         <v>13948</v>
       </c>
-      <c r="AT1" s="954" t="s">
+      <c r="AT1" s="1908" t="s">
         <v>13949</v>
       </c>
-      <c r="AU1" s="954" t="s">
+      <c r="AU1" s="1908" t="s">
         <v>13950</v>
       </c>
-      <c r="AV1" s="954" t="s">
+      <c r="AV1" s="1908" t="s">
         <v>13951</v>
       </c>
-      <c r="AW1" s="954" t="s">
+      <c r="AW1" s="1908" t="s">
         <v>13952</v>
       </c>
-      <c r="AX1" s="954" t="s">
+      <c r="AX1" s="1908" t="s">
         <v>13953</v>
       </c>
-      <c r="AY1" s="954" t="s">
+      <c r="AY1" s="1908" t="s">
         <v>13954</v>
       </c>
-      <c r="AZ1" s="954" t="s">
+      <c r="AZ1" s="1908" t="s">
         <v>13955</v>
       </c>
-      <c r="BA1" s="954" t="s">
+      <c r="BA1" s="1908" t="s">
         <v>13956</v>
       </c>
-      <c r="BB1" s="954" t="s">
+      <c r="BB1" s="1908" t="s">
         <v>13957</v>
       </c>
-      <c r="BC1" s="954" t="s">
+      <c r="BC1" s="1908" t="s">
         <v>13958</v>
       </c>
-      <c r="BD1" s="954" t="s">
+      <c r="BD1" s="1908" t="s">
         <v>13959</v>
       </c>
-      <c r="BE1" s="954" t="s">
+      <c r="BE1" s="1908" t="s">
         <v>13960</v>
       </c>
-      <c r="BF1" s="954" t="s">
+      <c r="BF1" s="1908" t="s">
         <v>13961</v>
       </c>
-      <c r="BG1" s="954" t="s">
+      <c r="BG1" s="1908" t="s">
         <v>13962</v>
       </c>
-      <c r="BH1" s="954" t="s">
+      <c r="BH1" s="1908" t="s">
         <v>13963</v>
       </c>
-      <c r="BI1" s="954" t="s">
+      <c r="BI1" s="1908" t="s">
         <v>13964</v>
       </c>
-      <c r="BJ1" s="954" t="s">
+      <c r="BJ1" s="1908" t="s">
         <v>13965</v>
       </c>
-      <c r="BK1" s="954" t="s">
+      <c r="BK1" s="1908" t="s">
         <v>13966</v>
       </c>
-      <c r="BL1" s="954" t="s">
+      <c r="BL1" s="1908" t="s">
         <v>13967</v>
       </c>
-      <c r="BM1" s="954" t="s">
+      <c r="BM1" s="1908" t="s">
         <v>13968</v>
       </c>
-      <c r="BN1" s="954" t="s">
+      <c r="BN1" s="1908" t="s">
         <v>13969</v>
       </c>
-      <c r="BO1" s="954" t="s">
+      <c r="BO1" s="1908" t="s">
         <v>13970</v>
       </c>
-      <c r="BP1" s="954" t="s">
+      <c r="BP1" s="1908" t="s">
         <v>13971</v>
       </c>
-      <c r="BQ1" s="954" t="s">
+      <c r="BQ1" s="1908" t="s">
         <v>13972</v>
       </c>
-      <c r="BR1" s="954" t="s">
+      <c r="BR1" s="1908" t="s">
         <v>13973</v>
       </c>
-      <c r="BS1" s="954" t="s">
+      <c r="BS1" s="1908" t="s">
         <v>13974</v>
       </c>
-      <c r="BT1" s="954" t="s">
+      <c r="BT1" s="1908" t="s">
         <v>13975</v>
       </c>
-      <c r="BU1" s="954" t="s">
+      <c r="BU1" s="1908" t="s">
         <v>13976</v>
       </c>
-      <c r="BV1" s="954" t="s">
+      <c r="BV1" s="1908" t="s">
         <v>13977</v>
       </c>
-      <c r="BW1" s="954" t="s">
+      <c r="BW1" s="1908" t="s">
         <v>13978</v>
       </c>
-      <c r="BX1" s="954" t="s">
+      <c r="BX1" s="1908" t="s">
         <v>13979</v>
       </c>
-      <c r="BY1" s="954" t="s">
+      <c r="BY1" s="1908" t="s">
         <v>13980</v>
       </c>
-      <c r="BZ1" s="954" t="s">
+      <c r="BZ1" s="1908" t="s">
         <v>13981</v>
       </c>
-      <c r="CA1" s="954" t="s">
+      <c r="CA1" s="1908" t="s">
         <v>13982</v>
       </c>
-      <c r="CB1" s="954" t="s">
+      <c r="CB1" s="1908" t="s">
         <v>13983</v>
       </c>
-      <c r="CC1" s="954" t="s">
+      <c r="CC1" s="1908" t="s">
         <v>13984</v>
       </c>
-      <c r="CD1" s="954" t="s">
+      <c r="CD1" s="1908" t="s">
         <v>13985</v>
       </c>
-      <c r="CE1" s="954" t="s">
+      <c r="CE1" s="1908" t="s">
         <v>13986</v>
       </c>
-      <c r="CF1" s="954" t="s">
+      <c r="CF1" s="1908" t="s">
         <v>13987</v>
       </c>
-      <c r="CG1" s="954" t="s">
+      <c r="CG1" s="1908" t="s">
         <v>13988</v>
       </c>
-      <c r="CH1" s="954" t="s">
+      <c r="CH1" s="1908" t="s">
         <v>13989</v>
       </c>
-      <c r="CI1" s="954" t="s">
+      <c r="CI1" s="1908" t="s">
         <v>13990</v>
       </c>
-      <c r="CJ1" s="954" t="s">
+      <c r="CJ1" s="1908" t="s">
         <v>13991</v>
       </c>
     </row>

</xml_diff>